<commit_message>
Fixed Drag Hero Bugsssssss
</commit_message>
<xml_diff>
--- a/FYP phase 1 分工.xlsx
+++ b/FYP phase 1 分工.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\FYPMobile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3CEA69-C7EA-45B8-B67A-8FA695AEA528}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90A2B80-9AAC-4D84-B42B-B6D9855D68CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{9B108708-2A4B-472A-8D96-7FDF5F58F78D}"/>
   </bookViews>
@@ -545,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0391F70D-23CB-433A-B6FA-0741B800E3ED}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -583,7 +583,9 @@
       <c r="D2" s="4">
         <v>0.5</v>
       </c>
-      <c r="E2" s="9"/>
+      <c r="E2" s="10">
+        <v>43909</v>
+      </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">

</xml_diff>